<commit_message>
Se reemplaza el método de vue.js por js por problemas al cargar los datos al momento de editar un embarque
</commit_message>
<xml_diff>
--- a/archivos/Distribucion semana 31.xlsx
+++ b/archivos/Distribucion semana 31.xlsx
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="47">
   <si>
     <t>FINCA</t>
   </si>
@@ -261,6 +261,9 @@
   </si>
   <si>
     <t>COREANO</t>
+  </si>
+  <si>
+    <t>¿Quisiera saber por qué sigue sucediendo que realizo una compra por internet en una plataforma no se me efectúa, sin embargo la descuentan? Segunda vez consecutiva que sucede en esta plataforma.</t>
   </si>
 </sst>
 </file>
@@ -366,7 +369,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -376,6 +379,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -440,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -550,28 +559,55 @@
     <xf numFmtId="3" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -889,7 +925,7 @@
   <dimension ref="A1:AH27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,14 +945,15 @@
     <col min="16" max="17" width="6.85546875" style="11" customWidth="1"/>
     <col min="18" max="18" width="7.28515625" style="11" customWidth="1"/>
     <col min="19" max="19" width="6.85546875" style="11" customWidth="1"/>
-    <col min="20" max="22" width="6.140625" style="11" customWidth="1"/>
-    <col min="23" max="23" width="6.7109375" style="11" customWidth="1"/>
+    <col min="20" max="21" width="6.140625" style="11" customWidth="1"/>
+    <col min="22" max="22" width="6.140625" style="42" customWidth="1"/>
+    <col min="23" max="23" width="6.7109375" style="42" customWidth="1"/>
     <col min="24" max="24" width="6.85546875" style="15" customWidth="1"/>
     <col min="25" max="25" width="5.85546875" style="11" customWidth="1"/>
     <col min="26" max="26" width="5.7109375" style="11" customWidth="1"/>
-    <col min="27" max="27" width="6" style="11" customWidth="1"/>
-    <col min="28" max="28" width="6.5703125" style="11" customWidth="1"/>
-    <col min="29" max="29" width="6" style="11" customWidth="1"/>
+    <col min="27" max="27" width="6" style="42" customWidth="1"/>
+    <col min="28" max="28" width="6.5703125" style="42" customWidth="1"/>
+    <col min="29" max="29" width="6" style="42" customWidth="1"/>
     <col min="30" max="31" width="7.28515625" style="11" customWidth="1"/>
     <col min="32" max="32" width="9.5703125" style="11" customWidth="1"/>
     <col min="33" max="33" width="13.42578125" style="11" customWidth="1"/>
@@ -2318,11 +2355,11 @@
       </c>
     </row>
     <row r="2" spans="1:34" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -2341,14 +2378,14 @@
       <c r="S2" s="8"/>
       <c r="T2" s="8"/>
       <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
+      <c r="V2" s="43"/>
+      <c r="W2" s="43"/>
       <c r="X2" s="17"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
+      <c r="AA2" s="50"/>
+      <c r="AB2" s="50"/>
+      <c r="AC2" s="50"/>
       <c r="AD2" s="1"/>
       <c r="AF2" s="19">
         <v>82</v>
@@ -2358,39 +2395,39 @@
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="39" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="27"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="43"/>
-      <c r="R3" s="43"/>
-      <c r="S3" s="43"/>
-      <c r="T3" s="43"/>
-      <c r="U3" s="43"/>
-      <c r="V3" s="43"/>
-      <c r="W3" s="43"/>
-      <c r="X3" s="43"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
+      <c r="S3" s="40"/>
+      <c r="T3" s="40"/>
+      <c r="U3" s="40"/>
+      <c r="V3" s="40"/>
+      <c r="W3" s="40"/>
+      <c r="X3" s="40"/>
       <c r="Y3" s="21"/>
       <c r="Z3" s="35"/>
-      <c r="AA3" s="35"/>
-      <c r="AB3" s="38"/>
-      <c r="AC3" s="38"/>
+      <c r="AA3" s="51"/>
+      <c r="AB3" s="51"/>
+      <c r="AC3" s="51"/>
       <c r="AD3" s="25"/>
-      <c r="AE3" s="42" t="s">
+      <c r="AE3" s="39" t="s">
         <v>1</v>
       </c>
       <c r="AF3" s="23">
@@ -2401,7 +2438,7 @@
       </c>
     </row>
     <row r="4" spans="1:34" s="12" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="28" t="s">
         <v>23</v>
       </c>
@@ -2462,10 +2499,10 @@
       <c r="U4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="V4" s="2" t="s">
+      <c r="V4" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="W4" s="44" t="s">
         <v>41</v>
       </c>
       <c r="X4" s="2" t="s">
@@ -2477,19 +2514,19 @@
       <c r="Z4" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="AA4" s="16" t="s">
+      <c r="AA4" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="AB4" s="16" t="s">
+      <c r="AB4" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="AC4" s="16" t="s">
+      <c r="AC4" s="52" t="s">
         <v>40</v>
       </c>
       <c r="AD4" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="AE4" s="42"/>
+      <c r="AE4" s="39"/>
       <c r="AF4" s="12">
         <v>20399</v>
       </c>
@@ -2561,10 +2598,10 @@
       <c r="U5" s="33">
         <v>1142</v>
       </c>
-      <c r="V5" s="33">
+      <c r="V5" s="45">
         <v>1365</v>
       </c>
-      <c r="W5" s="33">
+      <c r="W5" s="45">
         <v>1367</v>
       </c>
       <c r="X5" s="33">
@@ -2576,13 +2613,13 @@
       <c r="Z5" s="33">
         <v>1303</v>
       </c>
-      <c r="AA5" s="33">
+      <c r="AA5" s="45">
         <v>1366</v>
       </c>
-      <c r="AB5" s="33">
+      <c r="AB5" s="45">
         <v>1368</v>
       </c>
-      <c r="AC5" s="33">
+      <c r="AC5" s="45">
         <v>1373</v>
       </c>
       <c r="AD5" s="33">
@@ -2641,20 +2678,20 @@
       </c>
       <c r="T6" s="7"/>
       <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
+      <c r="V6" s="46"/>
+      <c r="W6" s="46"/>
       <c r="X6" s="3">
         <v>12</v>
       </c>
       <c r="Y6" s="7"/>
       <c r="Z6" s="7"/>
-      <c r="AA6" s="7">
+      <c r="AA6" s="46">
         <v>42</v>
       </c>
-      <c r="AB6" s="7">
+      <c r="AB6" s="46">
         <v>30</v>
       </c>
-      <c r="AC6" s="7">
+      <c r="AC6" s="46">
         <v>1392</v>
       </c>
       <c r="AD6" s="7">
@@ -2717,20 +2754,20 @@
         <v>16</v>
       </c>
       <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
+      <c r="V7" s="46"/>
+      <c r="W7" s="46"/>
       <c r="X7" s="3">
         <v>10</v>
       </c>
       <c r="Y7" s="7"/>
       <c r="Z7" s="7"/>
-      <c r="AA7" s="7">
+      <c r="AA7" s="46">
         <v>42</v>
       </c>
-      <c r="AB7" s="7">
+      <c r="AB7" s="46">
         <v>25</v>
       </c>
-      <c r="AC7" s="7">
+      <c r="AC7" s="46">
         <v>1152</v>
       </c>
       <c r="AD7" s="7">
@@ -2791,18 +2828,18 @@
       </c>
       <c r="T8" s="7"/>
       <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
+      <c r="V8" s="46"/>
+      <c r="W8" s="46"/>
       <c r="X8" s="3">
         <v>10</v>
       </c>
       <c r="Y8" s="7"/>
       <c r="Z8" s="7"/>
-      <c r="AA8" s="7">
+      <c r="AA8" s="46">
         <v>42</v>
       </c>
-      <c r="AB8" s="7"/>
-      <c r="AC8" s="7"/>
+      <c r="AB8" s="46"/>
+      <c r="AC8" s="46"/>
       <c r="AD8" s="7"/>
       <c r="AE8" s="3">
         <f t="shared" si="0"/>
@@ -2855,10 +2892,10 @@
       </c>
       <c r="T9" s="7"/>
       <c r="U9" s="7"/>
-      <c r="V9" s="7">
+      <c r="V9" s="46">
         <v>44</v>
       </c>
-      <c r="W9" s="39">
+      <c r="W9" s="49">
         <v>1344</v>
       </c>
       <c r="X9" s="3">
@@ -2868,11 +2905,11 @@
         <v>27</v>
       </c>
       <c r="Z9" s="7"/>
-      <c r="AA9" s="7">
+      <c r="AA9" s="46">
         <v>42</v>
       </c>
-      <c r="AB9" s="7"/>
-      <c r="AC9" s="7"/>
+      <c r="AB9" s="46"/>
+      <c r="AC9" s="46"/>
       <c r="AD9" s="7"/>
       <c r="AE9" s="3">
         <f t="shared" si="0"/>
@@ -2929,10 +2966,10 @@
       </c>
       <c r="T10" s="7"/>
       <c r="U10" s="7"/>
-      <c r="V10" s="7">
+      <c r="V10" s="46">
         <v>44</v>
       </c>
-      <c r="W10" s="7"/>
+      <c r="W10" s="46"/>
       <c r="X10" s="7">
         <v>20</v>
       </c>
@@ -2940,9 +2977,9 @@
       <c r="Z10" s="7">
         <v>84</v>
       </c>
-      <c r="AA10" s="7"/>
-      <c r="AB10" s="7"/>
-      <c r="AC10" s="7">
+      <c r="AA10" s="46"/>
+      <c r="AB10" s="46"/>
+      <c r="AC10" s="46">
         <v>2304</v>
       </c>
       <c r="AD10" s="7">
@@ -3001,8 +3038,8 @@
       <c r="U11" s="7">
         <v>17</v>
       </c>
-      <c r="V11" s="7"/>
-      <c r="W11" s="39">
+      <c r="V11" s="46"/>
+      <c r="W11" s="49">
         <v>816</v>
       </c>
       <c r="X11" s="7">
@@ -3010,9 +3047,9 @@
       </c>
       <c r="Y11" s="7"/>
       <c r="Z11" s="7"/>
-      <c r="AA11" s="7"/>
-      <c r="AB11" s="7"/>
-      <c r="AC11" s="7"/>
+      <c r="AA11" s="46"/>
+      <c r="AB11" s="46"/>
+      <c r="AC11" s="46"/>
       <c r="AD11" s="7"/>
       <c r="AE11" s="3">
         <f t="shared" si="0"/>
@@ -3107,11 +3144,11 @@
         <f>SUM(U6:U11)</f>
         <v>17</v>
       </c>
-      <c r="V12" s="20">
+      <c r="V12" s="47">
         <f>SUM(V6:V11)</f>
         <v>88</v>
       </c>
-      <c r="W12" s="20">
+      <c r="W12" s="47">
         <f>SUM(W6:W11)</f>
         <v>2160</v>
       </c>
@@ -3127,15 +3164,15 @@
         <f>SUM(Z6:Z11)</f>
         <v>84</v>
       </c>
-      <c r="AA12" s="20">
+      <c r="AA12" s="47">
         <f>SUM(AA6:AA11)</f>
         <v>168</v>
       </c>
-      <c r="AB12" s="20">
+      <c r="AB12" s="47">
         <f>SUM(AB6:AB11)</f>
         <v>55</v>
       </c>
-      <c r="AC12" s="20">
+      <c r="AC12" s="47">
         <f>SUM(AC6:AC11)</f>
         <v>4848</v>
       </c>
@@ -3163,35 +3200,40 @@
     <row r="13" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="44"/>
-      <c r="L13" s="44"/>
-      <c r="M13" s="44"/>
-      <c r="N13" s="44"/>
-      <c r="O13" s="44"/>
-      <c r="P13" s="44"/>
-      <c r="Q13" s="44"/>
-      <c r="R13" s="44"/>
-      <c r="S13" s="44"/>
-      <c r="T13" s="44"/>
-      <c r="U13" s="44"/>
-      <c r="V13" s="44"/>
-      <c r="W13" s="44"/>
-      <c r="X13" s="44"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="41"/>
+      <c r="R13" s="41"/>
+      <c r="S13" s="41"/>
+      <c r="T13" s="41"/>
+      <c r="U13" s="41"/>
+      <c r="V13" s="41"/>
+      <c r="W13" s="41"/>
+      <c r="X13" s="41"/>
       <c r="Y13" s="22"/>
       <c r="Z13" s="34"/>
-      <c r="AA13" s="34"/>
-      <c r="AB13" s="37"/>
-      <c r="AC13" s="37"/>
+      <c r="AA13" s="53"/>
+      <c r="AB13" s="53"/>
+      <c r="AC13" s="53"/>
       <c r="AD13" s="26"/>
       <c r="AE13" s="19"/>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="H15" s="11" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AF16" s="23">
@@ -3202,11 +3244,11 @@
       </c>
     </row>
     <row r="17" spans="1:34" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -3225,14 +3267,14 @@
       <c r="S17" s="8"/>
       <c r="T17" s="8"/>
       <c r="U17" s="8"/>
-      <c r="V17" s="8"/>
-      <c r="W17" s="8"/>
+      <c r="V17" s="43"/>
+      <c r="W17" s="43"/>
       <c r="X17" s="17"/>
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
-      <c r="AA17" s="1"/>
-      <c r="AB17" s="1"/>
-      <c r="AC17" s="1"/>
+      <c r="AA17" s="50"/>
+      <c r="AB17" s="50"/>
+      <c r="AC17" s="50"/>
       <c r="AD17" s="1"/>
       <c r="AF17" s="19">
         <v>82</v>
@@ -3242,39 +3284,39 @@
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="39" t="s">
         <v>0</v>
       </c>
       <c r="B18" s="27"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="43"/>
-      <c r="L18" s="43"/>
-      <c r="M18" s="43"/>
-      <c r="N18" s="43"/>
-      <c r="O18" s="43"/>
-      <c r="P18" s="43"/>
-      <c r="Q18" s="43"/>
-      <c r="R18" s="43"/>
-      <c r="S18" s="43"/>
-      <c r="T18" s="43"/>
-      <c r="U18" s="43"/>
-      <c r="V18" s="43"/>
-      <c r="W18" s="43"/>
-      <c r="X18" s="43"/>
-      <c r="Y18" s="40"/>
-      <c r="Z18" s="40"/>
-      <c r="AA18" s="40"/>
-      <c r="AB18" s="40"/>
-      <c r="AC18" s="40"/>
-      <c r="AD18" s="40"/>
-      <c r="AE18" s="42" t="s">
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="40"/>
+      <c r="O18" s="40"/>
+      <c r="P18" s="40"/>
+      <c r="Q18" s="40"/>
+      <c r="R18" s="40"/>
+      <c r="S18" s="40"/>
+      <c r="T18" s="40"/>
+      <c r="U18" s="40"/>
+      <c r="V18" s="40"/>
+      <c r="W18" s="40"/>
+      <c r="X18" s="40"/>
+      <c r="Y18" s="37"/>
+      <c r="Z18" s="37"/>
+      <c r="AA18" s="51"/>
+      <c r="AB18" s="51"/>
+      <c r="AC18" s="51"/>
+      <c r="AD18" s="37"/>
+      <c r="AE18" s="39" t="s">
         <v>1</v>
       </c>
       <c r="AF18" s="23">
@@ -3285,7 +3327,7 @@
       </c>
     </row>
     <row r="19" spans="1:34" s="12" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="42"/>
+      <c r="A19" s="39"/>
       <c r="B19" s="28" t="s">
         <v>23</v>
       </c>
@@ -3346,10 +3388,10 @@
       <c r="U19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="V19" s="2" t="s">
+      <c r="V19" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="W19" s="2" t="s">
+      <c r="W19" s="44" t="s">
         <v>41</v>
       </c>
       <c r="X19" s="2" t="s">
@@ -3361,19 +3403,19 @@
       <c r="Z19" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="AA19" s="16" t="s">
+      <c r="AA19" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="AB19" s="16" t="s">
+      <c r="AB19" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="AC19" s="16" t="s">
+      <c r="AC19" s="52" t="s">
         <v>40</v>
       </c>
       <c r="AD19" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="AE19" s="42"/>
+      <c r="AE19" s="39"/>
       <c r="AF19" s="12">
         <v>20399</v>
       </c>
@@ -3445,10 +3487,10 @@
       <c r="U20" s="14">
         <v>1142</v>
       </c>
-      <c r="V20" s="14">
+      <c r="V20" s="48">
         <v>1365</v>
       </c>
-      <c r="W20" s="14">
+      <c r="W20" s="48">
         <v>1367</v>
       </c>
       <c r="X20" s="14">
@@ -3460,13 +3502,13 @@
       <c r="Z20" s="14">
         <v>1303</v>
       </c>
-      <c r="AA20" s="14">
+      <c r="AA20" s="48">
         <v>1366</v>
       </c>
-      <c r="AB20" s="14">
+      <c r="AB20" s="48">
         <v>1368</v>
       </c>
-      <c r="AC20" s="14">
+      <c r="AC20" s="48">
         <v>1373</v>
       </c>
       <c r="AD20" s="14">
@@ -3525,20 +3567,20 @@
       </c>
       <c r="T21" s="7"/>
       <c r="U21" s="7"/>
-      <c r="V21" s="7"/>
-      <c r="W21" s="7"/>
+      <c r="V21" s="46"/>
+      <c r="W21" s="46"/>
       <c r="X21" s="3">
         <v>27</v>
       </c>
       <c r="Y21" s="7"/>
       <c r="Z21" s="7"/>
-      <c r="AA21" s="7">
+      <c r="AA21" s="46">
         <v>42</v>
       </c>
-      <c r="AB21" s="7">
+      <c r="AB21" s="46">
         <v>30</v>
       </c>
-      <c r="AC21" s="7">
+      <c r="AC21" s="46">
         <v>1392</v>
       </c>
       <c r="AD21" s="7">
@@ -3601,20 +3643,20 @@
         <v>16</v>
       </c>
       <c r="U22" s="7"/>
-      <c r="V22" s="7"/>
-      <c r="W22" s="7"/>
+      <c r="V22" s="46"/>
+      <c r="W22" s="46"/>
       <c r="X22" s="3">
         <v>25</v>
       </c>
       <c r="Y22" s="7"/>
       <c r="Z22" s="7"/>
-      <c r="AA22" s="7">
+      <c r="AA22" s="46">
         <v>42</v>
       </c>
-      <c r="AB22" s="7">
+      <c r="AB22" s="46">
         <v>25</v>
       </c>
-      <c r="AC22" s="7">
+      <c r="AC22" s="46">
         <v>1152</v>
       </c>
       <c r="AD22" s="7">
@@ -3673,18 +3715,18 @@
       </c>
       <c r="T23" s="7"/>
       <c r="U23" s="7"/>
-      <c r="V23" s="7"/>
-      <c r="W23" s="7"/>
+      <c r="V23" s="46"/>
+      <c r="W23" s="46"/>
       <c r="X23" s="3">
         <v>20</v>
       </c>
       <c r="Y23" s="7"/>
       <c r="Z23" s="7"/>
-      <c r="AA23" s="7">
+      <c r="AA23" s="46">
         <v>42</v>
       </c>
-      <c r="AB23" s="7"/>
-      <c r="AC23" s="7"/>
+      <c r="AB23" s="46"/>
+      <c r="AC23" s="46"/>
       <c r="AD23" s="7"/>
       <c r="AE23" s="3">
         <f t="shared" si="4"/>
@@ -3739,10 +3781,10 @@
       </c>
       <c r="T24" s="7"/>
       <c r="U24" s="7"/>
-      <c r="V24" s="7">
+      <c r="V24" s="46">
         <v>44</v>
       </c>
-      <c r="W24" s="7">
+      <c r="W24" s="46">
         <v>1344</v>
       </c>
       <c r="X24" s="3">
@@ -3752,11 +3794,11 @@
         <v>27</v>
       </c>
       <c r="Z24" s="7"/>
-      <c r="AA24" s="7">
+      <c r="AA24" s="46">
         <v>42</v>
       </c>
-      <c r="AB24" s="7"/>
-      <c r="AC24" s="7"/>
+      <c r="AB24" s="46"/>
+      <c r="AC24" s="46"/>
       <c r="AD24" s="7"/>
       <c r="AE24" s="3">
         <f t="shared" si="4"/>
@@ -3811,10 +3853,10 @@
       </c>
       <c r="T25" s="7"/>
       <c r="U25" s="7"/>
-      <c r="V25" s="7">
+      <c r="V25" s="46">
         <v>44</v>
       </c>
-      <c r="W25" s="7"/>
+      <c r="W25" s="46"/>
       <c r="X25" s="7">
         <v>40</v>
       </c>
@@ -3822,9 +3864,9 @@
       <c r="Z25" s="7">
         <v>84</v>
       </c>
-      <c r="AA25" s="7"/>
-      <c r="AB25" s="7"/>
-      <c r="AC25" s="7">
+      <c r="AA25" s="46"/>
+      <c r="AB25" s="46"/>
+      <c r="AC25" s="46">
         <v>2304</v>
       </c>
       <c r="AD25" s="7">
@@ -3881,8 +3923,8 @@
       <c r="U26" s="7">
         <v>17</v>
       </c>
-      <c r="V26" s="7"/>
-      <c r="W26" s="7">
+      <c r="V26" s="46"/>
+      <c r="W26" s="46">
         <v>816</v>
       </c>
       <c r="X26" s="7">
@@ -3890,9 +3932,9 @@
       </c>
       <c r="Y26" s="7"/>
       <c r="Z26" s="7"/>
-      <c r="AA26" s="7"/>
-      <c r="AB26" s="7"/>
-      <c r="AC26" s="7"/>
+      <c r="AA26" s="46"/>
+      <c r="AB26" s="46"/>
+      <c r="AC26" s="46"/>
       <c r="AD26" s="7"/>
       <c r="AE26" s="3">
         <f t="shared" si="4"/>
@@ -3987,11 +4029,11 @@
         <f>SUM(U21:U26)</f>
         <v>17</v>
       </c>
-      <c r="V27" s="20">
+      <c r="V27" s="47">
         <f>SUM(V21:V26)</f>
         <v>88</v>
       </c>
-      <c r="W27" s="20">
+      <c r="W27" s="47">
         <f>SUM(W21:W26)</f>
         <v>2160</v>
       </c>
@@ -4007,15 +4049,15 @@
         <f>SUM(Z21:Z26)</f>
         <v>84</v>
       </c>
-      <c r="AA27" s="20">
+      <c r="AA27" s="47">
         <f>SUM(AA21:AA26)</f>
         <v>168</v>
       </c>
-      <c r="AB27" s="20">
+      <c r="AB27" s="47">
         <f>SUM(AB21:AB26)</f>
         <v>55</v>
       </c>
-      <c r="AC27" s="20">
+      <c r="AC27" s="47">
         <f>SUM(AC21:AC26)</f>
         <v>4848</v>
       </c>

</xml_diff>